<commit_message>
- first login ask for genre and age
</commit_message>
<xml_diff>
--- a/purchases_dataset.xlsx
+++ b/purchases_dataset.xlsx
@@ -20,12 +20,30 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="8">
   <si>
     <t xml:space="preserve">user_id</t>
   </si>
   <si>
+    <t xml:space="preserve">username</t>
+  </si>
+  <si>
     <t xml:space="preserve">wine_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">angela</t>
+  </si>
+  <si>
+    <t xml:space="preserve">paco</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pedro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cairo</t>
   </si>
 </sst>
 </file>
@@ -58,12 +76,18 @@
       <family val="0"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFCC"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -100,7 +124,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -109,8 +133,12 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -236,10 +264,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:D36"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="310" zoomScaleNormal="310" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
+      <selection pane="topLeft" activeCell="E5" activeCellId="0" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -251,78 +279,307 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="n">
-        <v>8</v>
+      <c r="B2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D2" s="2" t="n">
+        <v>10256060181</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B3" s="1" t="n">
-        <v>10</v>
+      <c r="B3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="1" t="n">
+        <f aca="false">C2+1</f>
+        <v>1</v>
+      </c>
+      <c r="D3" s="2" t="n">
+        <v>10156060182</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B4" s="1" t="n">
-        <v>11</v>
+      <c r="B4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="1" t="n">
+        <f aca="false">C3+1</f>
+        <v>2</v>
+      </c>
+      <c r="D4" s="2" t="n">
+        <v>10234480185</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="B5" s="1" t="n">
-        <v>100</v>
+        <v>1</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="1" t="n">
+        <v>153</v>
+      </c>
+      <c r="D5" s="3" t="n">
+        <v>10133330283</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="B6" s="1" t="n">
-        <v>130</v>
+      <c r="B6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="1" t="n">
+        <f aca="false">C4+1</f>
+        <v>3</v>
+      </c>
+      <c r="D6" s="2" t="n">
+        <v>10434081882</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="B7" s="1" t="n">
-        <v>111</v>
+      <c r="B7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="1" t="n">
+        <f aca="false">C6+1</f>
+        <v>4</v>
+      </c>
+      <c r="D7" s="2" t="n">
+        <v>10434081881</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="B8" s="1" t="n">
-        <v>201</v>
+        <v>2</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="1" t="n">
+        <f aca="false">C7+1</f>
+        <v>5</v>
+      </c>
+      <c r="D8" s="2" t="n">
+        <v>10134270181</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="B9" s="1" t="n">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="2" t="n">
+      <c r="B9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="1" t="n">
+        <f aca="false">C8+1</f>
+        <v>6</v>
+      </c>
+      <c r="D9" s="2" t="n">
+        <v>10334270184</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="B10" s="1" t="n">
-        <v>123</v>
-      </c>
+      <c r="B10" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="1" t="n">
+        <f aca="false">C9+1</f>
+        <v>7</v>
+      </c>
+      <c r="D10" s="2" t="n">
+        <v>10234270185</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" s="1" t="n">
+        <f aca="false">C10+1</f>
+        <v>8</v>
+      </c>
+      <c r="D11" s="2" t="n">
+        <v>10134270183</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" s="1" t="n">
+        <f aca="false">C11+1</f>
+        <v>9</v>
+      </c>
+      <c r="D12" s="2" t="n">
+        <v>10234261083</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" s="1" t="n">
+        <f aca="false">C12+1</f>
+        <v>10</v>
+      </c>
+      <c r="D13" s="2" t="n">
+        <v>10134261084</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" s="1" t="n">
+        <f aca="false">C13+1</f>
+        <v>11</v>
+      </c>
+      <c r="D14" s="2" t="n">
+        <v>10134490483</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" s="1" t="n">
+        <f aca="false">C14+1</f>
+        <v>12</v>
+      </c>
+      <c r="D15" s="2" t="n">
+        <v>10134490283</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" s="1" t="n">
+        <f aca="false">C15+1</f>
+        <v>13</v>
+      </c>
+      <c r="D16" s="2" t="n">
+        <v>10134490282</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C17" s="1" t="n">
+        <f aca="false">C16+1</f>
+        <v>14</v>
+      </c>
+      <c r="D17" s="2" t="n">
+        <v>10134490281</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="D18" s="2"/>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="D19" s="2"/>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="D20" s="2"/>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="D21" s="2"/>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="D22" s="2"/>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="D23" s="2"/>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="D24" s="2"/>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="D25" s="2"/>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="D26" s="2"/>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="D27" s="2"/>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="D28" s="2"/>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="D29" s="2"/>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="D30" s="2"/>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="D31" s="2"/>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="D32" s="2"/>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="D33" s="2"/>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="D34" s="2"/>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="D35" s="2"/>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="D36" s="2"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>